<commit_message>
Edit and export Moreno Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/MorenoTasksAllocation.xlsx
+++ b/pp/gantt/MorenoTasksAllocation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Task #</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>Revision and requirement traceability</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>Integration test strategy</t>
+  </si>
+  <si>
+    <t>Definition of precedences</t>
+  </si>
+  <si>
+    <t>Sequence of components integration</t>
+  </si>
+  <si>
+    <t>Tools and equipment</t>
   </si>
 </sst>
 </file>
@@ -494,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +559,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D27" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
+        <f t="shared" ref="D2:D33" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
         <v>40g</v>
       </c>
       <c r="E2" s="2">
@@ -806,13 +821,13 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="E13" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F13" s="2">
-        <v>42687.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -830,13 +845,13 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="E14" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F14" s="2">
-        <v>42687.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G14">
         <v>3</v>
@@ -851,13 +866,13 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="E15" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F15" s="2">
-        <v>42685.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -868,31 +883,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>4g</v>
       </c>
       <c r="E16" s="2">
-        <v>42688.333333333336</v>
+        <v>42682.333333333336</v>
       </c>
       <c r="F16" s="2">
-        <v>42690.666666666664</v>
+        <v>42685.666666666664</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -908,15 +923,15 @@
         <v>42690.666666666664</v>
       </c>
       <c r="G17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -935,12 +950,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -959,194 +974,345 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>2g</v>
+        <v>3g</v>
       </c>
       <c r="E20" s="2">
-        <v>42691.333333333336</v>
+        <v>42688.333333333336</v>
       </c>
       <c r="F20" s="2">
-        <v>42692.666666666664</v>
+        <v>42690.666666666664</v>
       </c>
       <c r="G20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>1g</v>
       </c>
       <c r="E21" s="2">
-        <v>42695.333333333336</v>
+        <v>42691.333333333336</v>
       </c>
       <c r="F21" s="2">
-        <v>42697.666666666664</v>
+        <v>42691.666666666664</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>2g</v>
       </c>
       <c r="E22" s="2">
-        <v>42698.333333333336</v>
+        <v>42692.333333333336</v>
       </c>
       <c r="F22" s="2">
-        <v>42702.666666666664</v>
+        <v>42695.666666666664</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>2g</v>
       </c>
       <c r="E23" s="2">
-        <v>42703.333333333336</v>
+        <v>42696.333333333336</v>
       </c>
       <c r="F23" s="2">
-        <v>42704.666666666664</v>
+        <v>42697.666666666664</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>1g</v>
+        <v>2g</v>
       </c>
       <c r="E24" s="2">
-        <v>42705.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="F24" s="2">
-        <v>42705.666666666664</v>
+        <v>42699.666666666664</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>3g</v>
+        <f>CONCATENATE(NETWORKDAYS(E25,F25),"g")</f>
+        <v>1g</v>
       </c>
       <c r="E25" s="2">
-        <v>42706.333333333336</v>
+        <v>42702.333333333336</v>
       </c>
       <c r="F25" s="2">
-        <v>42710.666666666664</v>
+        <v>42702.666666666664</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>1g</v>
+        <f>CONCATENATE(NETWORKDAYS(E26,F26),"g")</f>
+        <v>2g</v>
       </c>
       <c r="E26" s="2">
-        <v>42711.333333333336</v>
+        <v>42703.333333333336</v>
       </c>
       <c r="F26" s="2">
-        <v>42711.666666666664</v>
+        <v>42704.666666666664</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E27" s="2">
+        <v>42705.333333333336</v>
+      </c>
+      <c r="F27" s="2">
+        <v>42705.666666666664</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" t="str">
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>1g</v>
       </c>
-      <c r="E27" s="2">
-        <v>42713.333333333336</v>
-      </c>
-      <c r="F27" s="2">
-        <v>42713.666666666664</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
+      <c r="E28" s="2">
+        <v>42706.333333333336</v>
+      </c>
+      <c r="F28" s="2">
+        <v>42706.666666666664</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E29" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F29" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E30" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F30" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>2g</v>
+      </c>
+      <c r="E31" s="2">
+        <v>42717.333333333336</v>
+      </c>
+      <c r="F31" s="2">
+        <v>42718.666666666664</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E32" s="2">
+        <v>42719.333333333336</v>
+      </c>
+      <c r="F32" s="2">
+        <v>42719.666666666664</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>2g</v>
+      </c>
+      <c r="E33" s="2">
+        <v>42720.333333333336</v>
+      </c>
+      <c r="F33" s="2">
+        <v>42723.666666666664</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>